<commit_message>
Emp v time surface output
</commit_message>
<xml_diff>
--- a/Optimisation_Spreadsheet_v3.xlsx
+++ b/Optimisation_Spreadsheet_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakeelsubratty/PycharmProjects/optimisation/venv/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BF3D8F-69D2-D14A-A106-931E1B4D5590}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91804796-27C3-7C4C-B1D6-2A98DCAB75CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{5A44FB99-32D9-7941-96CE-1A742DBA76D8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{5A44FB99-32D9-7941-96CE-1A742DBA76D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Employees!$A$1:$H$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Payrolls!$A$1:$L$1235</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7561" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7559" uniqueCount="1360">
   <si>
     <t>Employee</t>
   </si>
@@ -4529,7 +4529,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5359,8 +5359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9BA9D2-15BC-DE4B-B138-2CB506C7A197}">
   <dimension ref="A1:M1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A1086" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E1105" sqref="E1105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34194,8 +34194,8 @@
       <c r="D701" t="s">
         <v>1302</v>
       </c>
-      <c r="E701" t="s">
-        <v>1303</v>
+      <c r="E701" s="4">
+        <v>3</v>
       </c>
       <c r="F701" s="5">
         <f t="shared" si="33"/>
@@ -50891,8 +50891,8 @@
       <c r="D1105" t="s">
         <v>1302</v>
       </c>
-      <c r="E1105" t="s">
-        <v>1303</v>
+      <c r="E1105" s="4">
+        <v>3</v>
       </c>
       <c r="F1105" s="5">
         <f t="shared" si="53"/>

</xml_diff>